<commit_message>
Add specific validation for collection date so it can be a date or "not provided"
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet_fail.xlsx
+++ b/tests/resources/brokering/metadata_sheet_fail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D573F2BA-4154-EF49-9DFF-EE9D1872FD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8E6E04-840D-2B41-BE0B-700278137AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="768">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2480,6 +2480,9 @@
   </si>
   <si>
     <t>Greatest analysis ever3</t>
+  </si>
+  <si>
+    <t>Dote of collection</t>
   </si>
 </sst>
 </file>
@@ -3014,6 +3017,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3023,20 +3038,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3416,8 +3419,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1">
-      <c r="A1" s="67"/>
-      <c r="B1" s="67"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3426,10 +3429,10 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="69"/>
+      <c r="B2" s="64"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -3438,10 +3441,10 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="19">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="65" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="70"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -3462,8 +3465,8 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1">
-      <c r="A5" s="67"/>
-      <c r="B5" s="67"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -3484,10 +3487,10 @@
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -3496,8 +3499,8 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1">
-      <c r="A8" s="65"/>
-      <c r="B8" s="65"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -3518,8 +3521,8 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1">
-      <c r="A10" s="67"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -3528,10 +3531,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="70" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="68"/>
+      <c r="B11" s="70"/>
     </row>
     <row r="12" spans="1:8" ht="20">
       <c r="A12" s="25" t="s">
@@ -3587,28 +3590,28 @@
       <c r="B18"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="63"/>
+      <c r="B19" s="67"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="67"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="63"/>
+      <c r="B21" s="67"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="63"/>
+      <c r="B22" s="67"/>
     </row>
     <row r="23" spans="1:2" s="3" customFormat="1">
       <c r="A23" s="10"/>
@@ -3617,11 +3620,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3631,6 +3629,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -6753,8 +6756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA103" sqref="AA4:AB103"/>
+    <sheetView tabSelected="1" topLeftCell="P80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA103" sqref="AA103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -9330,8 +9333,8 @@
       <c r="M102" t="s">
         <v>548</v>
       </c>
-      <c r="AA102" s="32">
-        <v>43845</v>
+      <c r="AA102" s="32" t="s">
+        <v>767</v>
       </c>
       <c r="AB102" t="s">
         <v>515</v>
@@ -9353,8 +9356,8 @@
       <c r="M103" t="s">
         <v>548</v>
       </c>
-      <c r="AA103" s="32">
-        <v>43845</v>
+      <c r="AA103" t="s">
+        <v>515</v>
       </c>
       <c r="AB103" t="s">
         <v>515</v>
@@ -9376,7 +9379,7 @@
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Analysis alias" prompt="Must match an analysis alias provided in the &quot;ANALYSIS&quot; sheet_x000a_Multiple entries can be separated with a comma_x000a_e.g. analysis1,analysis2" sqref="A1:A3 A1000001:A1048576" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names must match those provided in the VCF file(s)" sqref="B1:B1048576 F1:F1048576" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Collection date" prompt="In the format yyyy-mm-dd" sqref="AA1:AA1048576" xr:uid="{00000000-0002-0000-0700-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Collection date" prompt="In the format yyyy-mm-dd" sqref="AA1:AA102 AA104:AA1048576" xr:uid="{00000000-0002-0000-0700-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Disable check for additional files  (#164)
* Disable check for additional file being present in the 30_valid directory

* Add specific validation for collection date so it can be a date or "not provided"
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet_fail.xlsx
+++ b/tests/resources/brokering/metadata_sheet_fail.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D573F2BA-4154-EF49-9DFF-EE9D1872FD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8E6E04-840D-2B41-BE0B-700278137AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="767">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="768">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2480,6 +2480,9 @@
   </si>
   <si>
     <t>Greatest analysis ever3</t>
+  </si>
+  <si>
+    <t>Dote of collection</t>
   </si>
 </sst>
 </file>
@@ -3014,6 +3017,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3023,20 +3038,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3416,8 +3419,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1">
-      <c r="A1" s="67"/>
-      <c r="B1" s="67"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3426,10 +3429,10 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="69"/>
+      <c r="B2" s="64"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -3438,10 +3441,10 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="19">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="65" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="70"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -3462,8 +3465,8 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1">
-      <c r="A5" s="67"/>
-      <c r="B5" s="67"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -3484,10 +3487,10 @@
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -3496,8 +3499,8 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1">
-      <c r="A8" s="65"/>
-      <c r="B8" s="65"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -3518,8 +3521,8 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1">
-      <c r="A10" s="67"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -3528,10 +3531,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="70" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="68"/>
+      <c r="B11" s="70"/>
     </row>
     <row r="12" spans="1:8" ht="20">
       <c r="A12" s="25" t="s">
@@ -3587,28 +3590,28 @@
       <c r="B18"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="63"/>
+      <c r="B19" s="67"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="67"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="63"/>
+      <c r="B21" s="67"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="63"/>
+      <c r="B22" s="67"/>
     </row>
     <row r="23" spans="1:2" s="3" customFormat="1">
       <c r="A23" s="10"/>
@@ -3617,11 +3620,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3631,6 +3629,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -6753,8 +6756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA103" sqref="AA4:AB103"/>
+    <sheetView tabSelected="1" topLeftCell="P80" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA103" sqref="AA103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -9330,8 +9333,8 @@
       <c r="M102" t="s">
         <v>548</v>
       </c>
-      <c r="AA102" s="32">
-        <v>43845</v>
+      <c r="AA102" s="32" t="s">
+        <v>767</v>
       </c>
       <c r="AB102" t="s">
         <v>515</v>
@@ -9353,8 +9356,8 @@
       <c r="M103" t="s">
         <v>548</v>
       </c>
-      <c r="AA103" s="32">
-        <v>43845</v>
+      <c r="AA103" t="s">
+        <v>515</v>
       </c>
       <c r="AB103" t="s">
         <v>515</v>
@@ -9376,7 +9379,7 @@
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Analysis alias" prompt="Must match an analysis alias provided in the &quot;ANALYSIS&quot; sheet_x000a_Multiple entries can be separated with a comma_x000a_e.g. analysis1,analysis2" sqref="A1:A3 A1000001:A1048576" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names must match those provided in the VCF file(s)" sqref="B1:B1048576 F1:F1048576" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Collection date" prompt="In the format yyyy-mm-dd" sqref="AA1:AA1048576" xr:uid="{00000000-0002-0000-0700-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Collection date" prompt="In the format yyyy-mm-dd" sqref="AA1:AA102 AA104:AA1048576" xr:uid="{00000000-0002-0000-0700-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Fix from submissions (#166)
* Reformat the archival notification text
* Make the brokering results overwrite previous results for everything but PROJECT
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet_fail.xlsx
+++ b/tests/resources/brokering/metadata_sheet_fail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8E6E04-840D-2B41-BE0B-700278137AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A005C77-BE8B-AF49-918C-95F74B9F5394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2482,7 +2482,7 @@
     <t>Greatest analysis ever3</t>
   </si>
   <si>
-    <t>Dote of collection</t>
+    <t>Date of collection</t>
   </si>
 </sst>
 </file>
@@ -3017,18 +3017,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3038,8 +3026,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3419,8 +3419,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1">
-      <c r="A1" s="63"/>
-      <c r="B1" s="63"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="67"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3429,10 +3429,10 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="64"/>
+      <c r="B2" s="69"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -3441,10 +3441,10 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="19">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="70" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="65"/>
+      <c r="B3" s="70"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -3465,8 +3465,8 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1">
-      <c r="A5" s="63"/>
-      <c r="B5" s="63"/>
+      <c r="A5" s="67"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -3487,10 +3487,10 @@
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="68"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -3499,8 +3499,8 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1">
-      <c r="A8" s="69"/>
-      <c r="B8" s="69"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -3521,8 +3521,8 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1">
-      <c r="A10" s="63"/>
-      <c r="B10" s="63"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -3531,10 +3531,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="68" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="70"/>
+      <c r="B11" s="68"/>
     </row>
     <row r="12" spans="1:8" ht="20">
       <c r="A12" s="25" t="s">
@@ -3590,28 +3590,28 @@
       <c r="B18"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="67" t="s">
+      <c r="A19" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="67"/>
+      <c r="B19" s="63"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="67"/>
+      <c r="B20" s="63"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="67" t="s">
+      <c r="A21" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="67"/>
+      <c r="B21" s="63"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="67" t="s">
+      <c r="A22" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="67"/>
+      <c r="B22" s="63"/>
     </row>
     <row r="23" spans="1:2" s="3" customFormat="1">
       <c r="A23" s="10"/>
@@ -3620,6 +3620,11 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3629,11 +3634,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -6757,7 +6757,7 @@
   <dimension ref="A1:AT103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA103" sqref="AA103"/>
+      <selection activeCell="AA102" sqref="AA102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Add check for ENA projects and Biosamples accession
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet_fail.xlsx
+++ b/tests/resources/brokering/metadata_sheet_fail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A005C77-BE8B-AF49-918C-95F74B9F5394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261FAFFF-AC3E-064D-BC27-B935A4BC9C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="770">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2458,9 +2458,6 @@
     <t>Sample 99</t>
   </si>
   <si>
-    <t>Sample 100</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -2483,6 +2480,15 @@
   </si>
   <si>
     <t>Date of collection</t>
+  </si>
+  <si>
+    <t>SAME000001</t>
+  </si>
+  <si>
+    <t>PRJEB00001,ASMXX00001</t>
+  </si>
+  <si>
+    <t>PRJEB50521</t>
   </si>
 </sst>
 </file>
@@ -5441,16 +5447,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>759</v>
+      </c>
+      <c r="B2" t="s">
         <v>760</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="60" t="s">
         <v>761</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="D2" s="61" t="s">
         <v>762</v>
-      </c>
-      <c r="D2" s="61" t="s">
-        <v>763</v>
       </c>
       <c r="E2" t="s">
         <v>554</v>
@@ -5630,8 +5636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -5715,6 +5721,12 @@
       </c>
       <c r="E2">
         <v>9606</v>
+      </c>
+      <c r="G2" t="s">
+        <v>769</v>
+      </c>
+      <c r="H2" t="s">
+        <v>768</v>
       </c>
     </row>
   </sheetData>
@@ -6144,7 +6156,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -6235,10 +6247,10 @@
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1">
       <c r="A3" s="62" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C3" t="s">
         <v>559</v>
@@ -6255,7 +6267,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="62" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C4" t="s">
         <v>559</v>
@@ -6756,8 +6768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA102" sqref="AA102"/>
+    <sheetView topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -9334,7 +9346,7 @@
         <v>548</v>
       </c>
       <c r="AA102" s="32" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="AB102" t="s">
         <v>515</v>
@@ -9344,17 +9356,11 @@
       <c r="A103" t="s">
         <v>558</v>
       </c>
-      <c r="F103" t="s">
+      <c r="B103" t="s">
         <v>659</v>
       </c>
-      <c r="G103" t="s">
-        <v>759</v>
-      </c>
-      <c r="L103">
-        <v>9606</v>
-      </c>
-      <c r="M103" t="s">
-        <v>548</v>
+      <c r="C103" t="s">
+        <v>767</v>
       </c>
       <c r="AA103" t="s">
         <v>515</v>
@@ -9378,7 +9384,7 @@
   <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Analysis alias" prompt="Must match an analysis alias provided in the &quot;ANALYSIS&quot; sheet_x000a_Multiple entries can be separated with a comma_x000a_e.g. analysis1,analysis2" sqref="A1:A3 A1000001:A1048576" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names must match those provided in the VCF file(s)" sqref="B1:B1048576 F1:F1048576" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names must match those provided in the VCF file(s)" sqref="F1:F1048576 C103 B1:B102 B104:B1048576" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Collection date" prompt="In the format yyyy-mm-dd" sqref="AA1:AA102 AA104:AA1048576" xr:uid="{00000000-0002-0000-0700-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
EVA-2514 - Add check for ENA projects and Biosamples accession (#173)
* Add check for ENA projects and Biosamples accession
* Fixes suggested in review
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet_fail.xlsx
+++ b/tests/resources/brokering/metadata_sheet_fail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A005C77-BE8B-AF49-918C-95F74B9F5394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261FAFFF-AC3E-064D-BC27-B935A4BC9C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="770">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2458,9 +2458,6 @@
     <t>Sample 99</t>
   </si>
   <si>
-    <t>Sample 100</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -2483,6 +2480,15 @@
   </si>
   <si>
     <t>Date of collection</t>
+  </si>
+  <si>
+    <t>SAME000001</t>
+  </si>
+  <si>
+    <t>PRJEB00001,ASMXX00001</t>
+  </si>
+  <si>
+    <t>PRJEB50521</t>
   </si>
 </sst>
 </file>
@@ -5441,16 +5447,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>759</v>
+      </c>
+      <c r="B2" t="s">
         <v>760</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="60" t="s">
         <v>761</v>
       </c>
-      <c r="C2" s="60" t="s">
+      <c r="D2" s="61" t="s">
         <v>762</v>
-      </c>
-      <c r="D2" s="61" t="s">
-        <v>763</v>
       </c>
       <c r="E2" t="s">
         <v>554</v>
@@ -5630,8 +5636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -5715,6 +5721,12 @@
       </c>
       <c r="E2">
         <v>9606</v>
+      </c>
+      <c r="G2" t="s">
+        <v>769</v>
+      </c>
+      <c r="H2" t="s">
+        <v>768</v>
       </c>
     </row>
   </sheetData>
@@ -6144,7 +6156,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -6235,10 +6247,10 @@
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1">
       <c r="A3" s="62" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B3" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C3" t="s">
         <v>559</v>
@@ -6255,7 +6267,7 @@
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="62" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C4" t="s">
         <v>559</v>
@@ -6756,8 +6768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AT103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P80" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA102" sqref="AA102"/>
+    <sheetView topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -9334,7 +9346,7 @@
         <v>548</v>
       </c>
       <c r="AA102" s="32" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="AB102" t="s">
         <v>515</v>
@@ -9344,17 +9356,11 @@
       <c r="A103" t="s">
         <v>558</v>
       </c>
-      <c r="F103" t="s">
+      <c r="B103" t="s">
         <v>659</v>
       </c>
-      <c r="G103" t="s">
-        <v>759</v>
-      </c>
-      <c r="L103">
-        <v>9606</v>
-      </c>
-      <c r="M103" t="s">
-        <v>548</v>
+      <c r="C103" t="s">
+        <v>767</v>
       </c>
       <c r="AA103" t="s">
         <v>515</v>
@@ -9378,7 +9384,7 @@
   <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Analysis alias" prompt="Must match an analysis alias provided in the &quot;ANALYSIS&quot; sheet_x000a_Multiple entries can be separated with a comma_x000a_e.g. analysis1,analysis2" sqref="A1:A3 A1000001:A1048576" xr:uid="{00000000-0002-0000-0700-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names must match those provided in the VCF file(s)" sqref="B1:B1048576 F1:F1048576" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Metadata and VCF" prompt="These sample names must match those provided in the VCF file(s)" sqref="F1:F1048576 C103 B1:B102 B104:B1048576" xr:uid="{00000000-0002-0000-0700-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Collection date" prompt="In the format yyyy-mm-dd" sqref="AA1:AA102 AA104:AA1048576" xr:uid="{00000000-0002-0000-0700-000002000000}"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Add check to raise duplicate analysis alias
</commit_message>
<xml_diff>
--- a/tests/resources/brokering/metadata_sheet_fail.xlsx
+++ b/tests/resources/brokering/metadata_sheet_fail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tcezard/PycharmProjects/eva-submission/tests/resources/brokering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{261FAFFF-AC3E-064D-BC27-B935A4BC9C79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E8EC731-1B8B-E343-B8D1-D98FEC466ECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25700" windowHeight="18100" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLEASE READ FIRST" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="770">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="771">
   <si>
     <t>PLEASE READ FIRST</t>
   </si>
@@ -2489,6 +2489,9 @@
   </si>
   <si>
     <t>PRJEB50521</t>
+  </si>
+  <si>
+    <t>Greatest analysis ever with a different name but same alias</t>
   </si>
 </sst>
 </file>
@@ -3023,6 +3026,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3032,20 +3047,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3425,8 +3428,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1">
-      <c r="A1" s="67"/>
-      <c r="B1" s="67"/>
+      <c r="A1" s="63"/>
+      <c r="B1" s="63"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -3435,10 +3438,10 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" s="3" customFormat="1" ht="26.25" customHeight="1">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="69"/>
+      <c r="B2" s="64"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -3447,10 +3450,10 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="1:8" s="3" customFormat="1" ht="19">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="65" t="s">
         <v>523</v>
       </c>
-      <c r="B3" s="70"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
@@ -3471,8 +3474,8 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" s="3" customFormat="1">
-      <c r="A5" s="67"/>
-      <c r="B5" s="67"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="63"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -3493,10 +3496,10 @@
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" s="3" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="64"/>
+      <c r="B7" s="68"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -3505,8 +3508,8 @@
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1">
-      <c r="A8" s="65"/>
-      <c r="B8" s="65"/>
+      <c r="A8" s="69"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -3527,8 +3530,8 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" s="3" customFormat="1">
-      <c r="A10" s="67"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="63"/>
+      <c r="B10" s="63"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -3537,10 +3540,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="19.5" customHeight="1">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="70" t="s">
         <v>518</v>
       </c>
-      <c r="B11" s="68"/>
+      <c r="B11" s="70"/>
     </row>
     <row r="12" spans="1:8" ht="20">
       <c r="A12" s="25" t="s">
@@ -3596,28 +3599,28 @@
       <c r="B18"/>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A19" s="63" t="s">
+      <c r="A19" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="63"/>
+      <c r="B19" s="67"/>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="67"/>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="63"/>
+      <c r="B21" s="67"/>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1">
-      <c r="A22" s="63" t="s">
+      <c r="A22" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="63"/>
+      <c r="B22" s="67"/>
     </row>
     <row r="23" spans="1:2" s="3" customFormat="1">
       <c r="A23" s="10"/>
@@ -3626,11 +3629,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="qXS9mSszo6ZK4PVLf2a4mgrLN9LTYf+uHOdaWY7gal7eLQi1TYc4PKeNVhIGj1PsRxEc/Fk3JaqC7G3YqwmFZQ==" saltValue="v8qTKlsQPInt8A+7GIueog==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
@@ -3640,6 +3638,11 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -5636,7 +5639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -6153,10 +6156,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -6282,6 +6285,26 @@
         <v>547</v>
       </c>
     </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="62" t="s">
+        <v>770</v>
+      </c>
+      <c r="B5" t="s">
+        <v>558</v>
+      </c>
+      <c r="C5" t="s">
+        <v>559</v>
+      </c>
+      <c r="D5" s="62" t="s">
+        <v>553</v>
+      </c>
+      <c r="E5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F5" t="s">
+        <v>547</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="23" type="noConversion"/>
   <dataValidations count="1">
@@ -6296,7 +6319,7 @@
           <x14:formula1>
             <xm:f>Project!$A$2</xm:f>
           </x14:formula1>
-          <xm:sqref>D1 D5:D1048576</xm:sqref>
+          <xm:sqref>D1 D6:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000002000000}">
           <x14:formula1>

</xml_diff>